<commit_message>
added db to track insertion information
</commit_message>
<xml_diff>
--- a/data/map.xlsx
+++ b/data/map.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="68">
   <si>
     <t>TONOMETRIA</t>
   </si>
@@ -70,7 +70,7 @@
     <t>Consulta</t>
   </si>
   <si>
-    <t>Eliane Helena Francisco Gaspar</t>
+    <t>Wilson Helena Francisco Gaspar</t>
   </si>
   <si>
     <t>935592470</t>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>1|10</t>
+  </si>
+  <si>
+    <t>Eliane Helena Francisco Gaspar</t>
   </si>
   <si>
     <t>(-) 1|10</t>
@@ -224,7 +227,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -279,6 +282,12 @@
     </font>
     <font>
       <color rgb="FF000000"/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <family val="2"/>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
     </font>
@@ -590,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -684,6 +693,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8582,7 +8594,7 @@
   <dimension ref="A1:AK1000"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="12.5703125"/>
@@ -8866,9 +8878,15 @@
       <c r="A8" s="29">
         <v>2</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
+      <c r="B8" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>19</v>
+      </c>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
@@ -8878,7 +8896,9 @@
       <c r="K8" s="32"/>
       <c r="L8" s="32"/>
       <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
+      <c r="N8" s="31" t="s">
+        <v>20</v>
+      </c>
       <c r="O8" s="33"/>
       <c r="P8" s="33"/>
       <c r="Q8" s="33"/>
@@ -8906,16 +8926,16 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AB8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AD8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -8962,16 +8982,16 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AD9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9018,16 +9038,16 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AB10" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AD10" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9074,16 +9094,16 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AB11" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AD11" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9130,16 +9150,16 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AB12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AD12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9157,7 +9177,7 @@
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
+      <c r="M13" s="37"/>
       <c r="N13" s="31"/>
       <c r="O13" s="33"/>
       <c r="P13" s="33"/>
@@ -9186,16 +9206,16 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AB13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AD13" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9213,12 +9233,12 @@
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
-      <c r="M14" s="37"/>
+      <c r="M14" s="38"/>
       <c r="N14" s="31"/>
       <c r="O14" s="33"/>
       <c r="P14" s="33"/>
       <c r="Q14" s="33"/>
-      <c r="R14" s="37"/>
+      <c r="R14" s="38"/>
       <c r="S14" s="31" t="str">
         <f t="shared" ref="S14:V14" si="8">IF(OR(G14=$Z$7,G14=$Z$8,G14=$Z$9,G14=$Z$10,G14=$Z$11,G14=$Z$12,G14=$Z$13,G14=$Z$14,G14=$Z$15,G14=$Z$16,G14=$Z$17),"OFT",IF(OR(G14=$Z$33,G14=$Z$34,G14=$Z$35,$Z$31),"X","OPT"))</f>
         <v>OPT</v>
@@ -9242,16 +9262,16 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB14" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD14" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9298,16 +9318,16 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AB15" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AD15" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9354,16 +9374,16 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB16" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD16" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9410,16 +9430,16 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AA17" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AB17" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AD17" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9466,16 +9486,16 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA18" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB18" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AD18" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9522,16 +9542,16 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AA19" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB19" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD19" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -9578,13 +9598,13 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AA20" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AB20" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9631,16 +9651,16 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AA21" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AB21" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AD21" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9687,16 +9707,16 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AA22" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AB22" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AD22" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9743,16 +9763,16 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AA23" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AB23" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AD23" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -9799,16 +9819,16 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AA24" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AB24" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AD24" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -9943,16 +9963,16 @@
       <c r="X27" s="1"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AA27" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AB27" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AD27" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -9999,13 +10019,13 @@
       <c r="X28" s="1"/>
       <c r="Y28" s="2"/>
       <c r="Z28" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AA28" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AB28" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -10052,13 +10072,13 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AA29" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AB29" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -10105,13 +10125,13 @@
       <c r="X30" s="1"/>
       <c r="Y30" s="2"/>
       <c r="Z30" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA30" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AB30" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -10158,13 +10178,13 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AA31" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AB31" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -10211,13 +10231,13 @@
       <c r="X32" s="1"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA32" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB32" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -10264,13 +10284,13 @@
       <c r="X33" s="1"/>
       <c r="Y33" s="2"/>
       <c r="Z33" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA33" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AB33" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -10317,13 +10337,13 @@
       <c r="X34" s="1"/>
       <c r="Y34" s="2"/>
       <c r="Z34" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AA34" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB34" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -10370,13 +10390,13 @@
       <c r="X35" s="1"/>
       <c r="Y35" s="2"/>
       <c r="Z35" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AA35" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AB35" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -19144,43 +19164,43 @@
       <c r="Y211" s="2"/>
     </row>
     <row r="212" ht="14.25" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A212" s="38">
+      <c r="A212" s="39">
         <v>206</v>
       </c>
-      <c r="B212" s="39"/>
-      <c r="C212" s="40"/>
-      <c r="D212" s="40"/>
-      <c r="E212" s="40"/>
-      <c r="F212" s="40"/>
-      <c r="G212" s="40"/>
-      <c r="H212" s="40"/>
-      <c r="I212" s="40"/>
-      <c r="J212" s="40"/>
-      <c r="K212" s="40"/>
-      <c r="L212" s="40"/>
-      <c r="M212" s="40"/>
-      <c r="N212" s="40"/>
-      <c r="O212" s="41"/>
-      <c r="P212" s="41"/>
-      <c r="Q212" s="41"/>
-      <c r="R212" s="40"/>
-      <c r="S212" s="40" t="str">
+      <c r="B212" s="40"/>
+      <c r="C212" s="41"/>
+      <c r="D212" s="41"/>
+      <c r="E212" s="41"/>
+      <c r="F212" s="41"/>
+      <c r="G212" s="41"/>
+      <c r="H212" s="41"/>
+      <c r="I212" s="41"/>
+      <c r="J212" s="41"/>
+      <c r="K212" s="41"/>
+      <c r="L212" s="41"/>
+      <c r="M212" s="41"/>
+      <c r="N212" s="41"/>
+      <c r="O212" s="42"/>
+      <c r="P212" s="42"/>
+      <c r="Q212" s="42"/>
+      <c r="R212" s="41"/>
+      <c r="S212" s="41" t="str">
         <f t="shared" ref="S212:V212" si="206">IF(OR(G212=$Z$7,G212=$Z$8,G212=$Z$9,G212=$Z$10,G212=$Z$11,G212=$Z$12,G212=$Z$13,G212=$Z$14,G212=$Z$15,G212=$Z$16,G212=$Z$17),"OFT",IF(OR(G212=$Z$33,G212=$Z$34,G212=$Z$35,$Z$31),"X","OPT"))</f>
         <v>OPT</v>
       </c>
-      <c r="T212" s="40" t="str">
+      <c r="T212" s="41" t="str">
         <f t="shared" si="206"/>
         <v>OPT</v>
       </c>
-      <c r="U212" s="40" t="str">
+      <c r="U212" s="41" t="str">
         <f t="shared" si="206"/>
         <v>OPT</v>
       </c>
-      <c r="V212" s="40" t="str">
+      <c r="V212" s="41" t="str">
         <f t="shared" si="206"/>
         <v>OPT</v>
       </c>
-      <c r="W212" s="42" t="str">
+      <c r="W212" s="43" t="str">
         <f t="shared" si="1"/>
         <v>Optometria</v>
       </c>
@@ -19189,13 +19209,13 @@
     </row>
     <row r="213" ht="14.25" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B213" t="s">
         <v>19</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>18</v>
@@ -19204,34 +19224,34 @@
         <v>20</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O213" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P213" s="1"/>
       <c r="Q213" s="1"/>

</xml_diff>